<commit_message>
(C)    new Rob lift set additions, in progress
</commit_message>
<xml_diff>
--- a/Suppl/Plan 2.0 - lifting.xlsx
+++ b/Suppl/Plan 2.0 - lifting.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="170">
   <si>
     <t>Day 1</t>
   </si>
@@ -476,12 +476,78 @@
   </si>
   <si>
     <t>Couch Stretch</t>
+  </si>
+  <si>
+    <t>(Isometric Rear Delt Fly)</t>
+  </si>
+  <si>
+    <t>(Barbell Bench Press, Incline Overhand)</t>
+  </si>
+  <si>
+    <t>(Selectorized Shoulder Press, Reverse Grip)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Bench Press, Incline Overhand)</t>
+  </si>
+  <si>
+    <t>(Single-Arm Cable Triceps Extension, Standing, Facing)</t>
+  </si>
+  <si>
+    <t>(Bodyweight Crunch, Bicycle)</t>
+  </si>
+  <si>
+    <t>(Couch Stretch)</t>
+  </si>
+  <si>
+    <t>(Bench Squat Jumps)</t>
+  </si>
+  <si>
+    <t>3x8-10</t>
+  </si>
+  <si>
+    <t>Bodyweighht*Bodyweight (G)</t>
+  </si>
+  <si>
+    <t>Leg Press</t>
+  </si>
+  <si>
+    <t>Barbell Squat</t>
+  </si>
+  <si>
+    <t>(Barbell Squat)</t>
+  </si>
+  <si>
+    <t>(Static V-Hold)</t>
+  </si>
+  <si>
+    <t>(Selectorized Leg Press)</t>
+  </si>
+  <si>
+    <t>(Lunge Step Backs, On Rail)</t>
+  </si>
+  <si>
+    <t>(Steps, Doubles)</t>
+  </si>
+  <si>
+    <t>(Stability Ball Wall Squats)</t>
+  </si>
+  <si>
+    <t>(Selectorized Individual Leg Curls)</t>
+  </si>
+  <si>
+    <t>2x15</t>
+  </si>
+  <si>
+    <t>(Bosu Ball Dumbbell Squat)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -582,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -632,6 +698,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -641,25 +711,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,10 +1094,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="32">
         <v>42711</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1067,7 +1143,7 @@
       <c r="Q4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="R4" s="31" t="s">
+      <c r="R4" s="33" t="s">
         <v>103</v>
       </c>
       <c r="S4" t="s">
@@ -1103,7 +1179,7 @@
       <c r="Q5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R5" s="31"/>
+      <c r="R5" s="33"/>
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1120,7 +1196,7 @@
       <c r="Q6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R6" s="31"/>
+      <c r="R6" s="33"/>
       <c r="S6" t="s">
         <v>106</v>
       </c>
@@ -1140,7 +1216,7 @@
       <c r="Q7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="31" t="s">
+      <c r="R7" s="33" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1158,7 +1234,7 @@
       <c r="Q8" s="15">
         <v>3</v>
       </c>
-      <c r="R8" s="31"/>
+      <c r="R8" s="33"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1176,7 +1252,7 @@
       <c r="Q9" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R9" s="31" t="s">
+      <c r="R9" s="33" t="s">
         <v>103</v>
       </c>
       <c r="S9" t="s">
@@ -1200,7 +1276,7 @@
       <c r="Q10" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R10" s="31"/>
+      <c r="R10" s="33"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1217,7 +1293,7 @@
       <c r="Q11" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R11" s="31"/>
+      <c r="R11" s="33"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1454,20 +1530,20 @@
       <c r="Q32" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="S32" s="29" t="s">
+      <c r="S32" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="T32" s="29"/>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
       <c r="W32" s="27"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="29"/>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
+      <c r="S33" s="31"/>
+      <c r="T33" s="31"/>
+      <c r="U33" s="31"/>
+      <c r="V33" s="31"/>
       <c r="W33" s="27"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
@@ -1609,10 +1685,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,16 +1698,16 @@
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>129</v>
       </c>
       <c r="C1" s="15"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>101</v>
       </c>
@@ -1639,373 +1715,451 @@
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="J4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>104</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>162</v>
+      </c>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="J6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="6" t="s">
+      <c r="D7" s="41"/>
+      <c r="E7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="J7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D8" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="E8" s="21"/>
+      <c r="J8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="21"/>
+      <c r="J9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C10" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D10" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E10" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="D11" s="35"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="J11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="J12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C16" s="15"/>
+      <c r="F16">
+        <v>178.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="C17" s="15"/>
+      <c r="F17">
+        <f>14.7/100</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C18" s="15"/>
+      <c r="F18" s="42">
+        <f>F16*F17</f>
+        <v>26.2836</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="12"/>
+      <c r="F19" s="42">
+        <f>F16-F18</f>
+        <v>152.5164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="E20" s="17" t="s">
+      <c r="C21" s="15"/>
+      <c r="E21" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="C27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C28" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D28" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="J28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C29" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="D29" s="36"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="J29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D30" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="J30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="D31" s="35"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="J31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C32" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D32" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="J32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="37" t="s">
+      <c r="D33" s="35"/>
+      <c r="E33" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="18"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="J33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="18"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D35" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E35" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="J35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+      <c r="D36" s="36"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="J36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="C37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="15"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+      <c r="C40" s="15"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="15"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C42" s="15"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C43" s="15"/>
     </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E32:H33"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D34:D35"/>
+  <mergeCells count="7">
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E33:H34"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2052,10 +2206,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="32">
         <v>42711</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>

</xml_diff>

<commit_message>
(+)    Anterior Day II addition, in progress. won't publish until        more content is generated
</commit_message>
<xml_diff>
--- a/Suppl/Plan 2.0 - lifting.xlsx
+++ b/Suppl/Plan 2.0 - lifting.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jan Plan '16 - r0" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
-    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId3"/>
+    <sheet name="Anterior DayII" sheetId="10" r:id="rId3"/>
+    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$41</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="182">
   <si>
     <t>Day 1</t>
   </si>
@@ -539,6 +540,54 @@
   </si>
   <si>
     <t>(Bosu Ball Dumbbell Squat)</t>
+  </si>
+  <si>
+    <t>Moving through space</t>
+  </si>
+  <si>
+    <t>Iso-Lateral Incline Press (Arched Spine Endurance)</t>
+  </si>
+  <si>
+    <t>3x12 -&gt; 4x20</t>
+  </si>
+  <si>
+    <t>&lt;- start @ 20 lbs</t>
+  </si>
+  <si>
+    <t>Rear Facing Iso-Lateral Shoulder Press</t>
+  </si>
+  <si>
+    <t>Any Tricep Exercise</t>
+  </si>
+  <si>
+    <r>
+      <t>3x12</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;- Your choice! (Thoughts - Narrow Grip Press, Rope Extension)</t>
+  </si>
+  <si>
+    <t>Bench Hops with Foot Release</t>
+  </si>
+  <si>
+    <t>3x12 -&gt; 3x20</t>
+  </si>
+  <si>
+    <t>Bicycle Crunches</t>
+  </si>
+  <si>
+    <t>3x30</t>
   </si>
 </sst>
 </file>
@@ -548,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,16 +658,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -644,11 +726,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -702,30 +821,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -736,6 +831,44 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,10 +1227,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="36">
         <v>42711</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1143,7 +1276,7 @@
       <c r="Q4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="R4" s="33" t="s">
+      <c r="R4" s="37" t="s">
         <v>103</v>
       </c>
       <c r="S4" t="s">
@@ -1179,7 +1312,7 @@
       <c r="Q5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R5" s="33"/>
+      <c r="R5" s="37"/>
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1196,7 +1329,7 @@
       <c r="Q6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R6" s="33"/>
+      <c r="R6" s="37"/>
       <c r="S6" t="s">
         <v>106</v>
       </c>
@@ -1216,7 +1349,7 @@
       <c r="Q7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="33" t="s">
+      <c r="R7" s="37" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1234,7 +1367,7 @@
       <c r="Q8" s="15">
         <v>3</v>
       </c>
-      <c r="R8" s="33"/>
+      <c r="R8" s="37"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1252,7 +1385,7 @@
       <c r="Q9" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R9" s="33" t="s">
+      <c r="R9" s="37" t="s">
         <v>103</v>
       </c>
       <c r="S9" t="s">
@@ -1276,7 +1409,7 @@
       <c r="Q10" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R10" s="33"/>
+      <c r="R10" s="37"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1293,7 +1426,7 @@
       <c r="Q11" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R11" s="33"/>
+      <c r="R11" s="37"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1530,20 +1663,20 @@
       <c r="Q32" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="S32" s="31" t="s">
+      <c r="S32" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="T32" s="31"/>
-      <c r="U32" s="31"/>
-      <c r="V32" s="31"/>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
+      <c r="V32" s="35"/>
       <c r="W32" s="27"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="31"/>
-      <c r="U33" s="31"/>
-      <c r="V33" s="31"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="35"/>
       <c r="W33" s="27"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
@@ -1687,8 +1820,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B12"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1855,7 @@
       <c r="C4" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="31" t="s">
         <v>103</v>
       </c>
       <c r="E4" s="30" t="s">
@@ -1756,7 +1889,7 @@
       <c r="C6" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="21" t="s">
         <v>158</v>
       </c>
@@ -1774,7 +1907,7 @@
       <c r="C7" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="6" t="s">
         <v>106</v>
       </c>
@@ -1792,7 +1925,7 @@
       <c r="C8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="38" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="21"/>
@@ -1807,7 +1940,7 @@
       <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="21"/>
       <c r="J9" t="s">
         <v>165</v>
@@ -1820,7 +1953,7 @@
       <c r="C10" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="40" t="s">
         <v>103</v>
       </c>
       <c r="E10" s="30" t="s">
@@ -1840,7 +1973,7 @@
       <c r="C11" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -1856,7 +1989,7 @@
       <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1907,7 +2040,7 @@
         <v>108</v>
       </c>
       <c r="C18" s="15"/>
-      <c r="F18" s="42">
+      <c r="F18" s="34">
         <f>F16*F17</f>
         <v>26.2836</v>
       </c>
@@ -1918,7 +2051,7 @@
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="12"/>
-      <c r="F19" s="42">
+      <c r="F19" s="34">
         <f>F16-F18</f>
         <v>152.5164</v>
       </c>
@@ -1972,7 +2105,7 @@
       <c r="C28" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="40" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="30"/>
@@ -1990,7 +2123,7 @@
       <c r="C29" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2006,7 +2139,7 @@
       <c r="C30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="40" t="s">
         <v>103</v>
       </c>
       <c r="E30" s="30"/>
@@ -2024,7 +2157,7 @@
       <c r="C31" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -2040,7 +2173,7 @@
       <c r="C32" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="40" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="30"/>
@@ -2058,24 +2191,24 @@
       <c r="C33" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="37" t="s">
+      <c r="D33" s="38"/>
+      <c r="E33" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
       <c r="J33" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C34" s="18"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -2084,7 +2217,7 @@
       <c r="C35" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="38" t="s">
         <v>103</v>
       </c>
       <c r="E35" s="21" t="s">
@@ -2104,7 +2237,7 @@
       <c r="C36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="36"/>
+      <c r="D36" s="39"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -2167,6 +2300,326 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" customWidth="1"/>
+    <col min="260" max="260" width="26.7109375" customWidth="1"/>
+    <col min="261" max="261" width="17.140625" customWidth="1"/>
+    <col min="262" max="262" width="57.7109375" customWidth="1"/>
+    <col min="516" max="516" width="26.7109375" customWidth="1"/>
+    <col min="517" max="517" width="17.140625" customWidth="1"/>
+    <col min="518" max="518" width="57.7109375" customWidth="1"/>
+    <col min="772" max="772" width="26.7109375" customWidth="1"/>
+    <col min="773" max="773" width="17.140625" customWidth="1"/>
+    <col min="774" max="774" width="57.7109375" customWidth="1"/>
+    <col min="1028" max="1028" width="26.7109375" customWidth="1"/>
+    <col min="1029" max="1029" width="17.140625" customWidth="1"/>
+    <col min="1030" max="1030" width="57.7109375" customWidth="1"/>
+    <col min="1284" max="1284" width="26.7109375" customWidth="1"/>
+    <col min="1285" max="1285" width="17.140625" customWidth="1"/>
+    <col min="1286" max="1286" width="57.7109375" customWidth="1"/>
+    <col min="1540" max="1540" width="26.7109375" customWidth="1"/>
+    <col min="1541" max="1541" width="17.140625" customWidth="1"/>
+    <col min="1542" max="1542" width="57.7109375" customWidth="1"/>
+    <col min="1796" max="1796" width="26.7109375" customWidth="1"/>
+    <col min="1797" max="1797" width="17.140625" customWidth="1"/>
+    <col min="1798" max="1798" width="57.7109375" customWidth="1"/>
+    <col min="2052" max="2052" width="26.7109375" customWidth="1"/>
+    <col min="2053" max="2053" width="17.140625" customWidth="1"/>
+    <col min="2054" max="2054" width="57.7109375" customWidth="1"/>
+    <col min="2308" max="2308" width="26.7109375" customWidth="1"/>
+    <col min="2309" max="2309" width="17.140625" customWidth="1"/>
+    <col min="2310" max="2310" width="57.7109375" customWidth="1"/>
+    <col min="2564" max="2564" width="26.7109375" customWidth="1"/>
+    <col min="2565" max="2565" width="17.140625" customWidth="1"/>
+    <col min="2566" max="2566" width="57.7109375" customWidth="1"/>
+    <col min="2820" max="2820" width="26.7109375" customWidth="1"/>
+    <col min="2821" max="2821" width="17.140625" customWidth="1"/>
+    <col min="2822" max="2822" width="57.7109375" customWidth="1"/>
+    <col min="3076" max="3076" width="26.7109375" customWidth="1"/>
+    <col min="3077" max="3077" width="17.140625" customWidth="1"/>
+    <col min="3078" max="3078" width="57.7109375" customWidth="1"/>
+    <col min="3332" max="3332" width="26.7109375" customWidth="1"/>
+    <col min="3333" max="3333" width="17.140625" customWidth="1"/>
+    <col min="3334" max="3334" width="57.7109375" customWidth="1"/>
+    <col min="3588" max="3588" width="26.7109375" customWidth="1"/>
+    <col min="3589" max="3589" width="17.140625" customWidth="1"/>
+    <col min="3590" max="3590" width="57.7109375" customWidth="1"/>
+    <col min="3844" max="3844" width="26.7109375" customWidth="1"/>
+    <col min="3845" max="3845" width="17.140625" customWidth="1"/>
+    <col min="3846" max="3846" width="57.7109375" customWidth="1"/>
+    <col min="4100" max="4100" width="26.7109375" customWidth="1"/>
+    <col min="4101" max="4101" width="17.140625" customWidth="1"/>
+    <col min="4102" max="4102" width="57.7109375" customWidth="1"/>
+    <col min="4356" max="4356" width="26.7109375" customWidth="1"/>
+    <col min="4357" max="4357" width="17.140625" customWidth="1"/>
+    <col min="4358" max="4358" width="57.7109375" customWidth="1"/>
+    <col min="4612" max="4612" width="26.7109375" customWidth="1"/>
+    <col min="4613" max="4613" width="17.140625" customWidth="1"/>
+    <col min="4614" max="4614" width="57.7109375" customWidth="1"/>
+    <col min="4868" max="4868" width="26.7109375" customWidth="1"/>
+    <col min="4869" max="4869" width="17.140625" customWidth="1"/>
+    <col min="4870" max="4870" width="57.7109375" customWidth="1"/>
+    <col min="5124" max="5124" width="26.7109375" customWidth="1"/>
+    <col min="5125" max="5125" width="17.140625" customWidth="1"/>
+    <col min="5126" max="5126" width="57.7109375" customWidth="1"/>
+    <col min="5380" max="5380" width="26.7109375" customWidth="1"/>
+    <col min="5381" max="5381" width="17.140625" customWidth="1"/>
+    <col min="5382" max="5382" width="57.7109375" customWidth="1"/>
+    <col min="5636" max="5636" width="26.7109375" customWidth="1"/>
+    <col min="5637" max="5637" width="17.140625" customWidth="1"/>
+    <col min="5638" max="5638" width="57.7109375" customWidth="1"/>
+    <col min="5892" max="5892" width="26.7109375" customWidth="1"/>
+    <col min="5893" max="5893" width="17.140625" customWidth="1"/>
+    <col min="5894" max="5894" width="57.7109375" customWidth="1"/>
+    <col min="6148" max="6148" width="26.7109375" customWidth="1"/>
+    <col min="6149" max="6149" width="17.140625" customWidth="1"/>
+    <col min="6150" max="6150" width="57.7109375" customWidth="1"/>
+    <col min="6404" max="6404" width="26.7109375" customWidth="1"/>
+    <col min="6405" max="6405" width="17.140625" customWidth="1"/>
+    <col min="6406" max="6406" width="57.7109375" customWidth="1"/>
+    <col min="6660" max="6660" width="26.7109375" customWidth="1"/>
+    <col min="6661" max="6661" width="17.140625" customWidth="1"/>
+    <col min="6662" max="6662" width="57.7109375" customWidth="1"/>
+    <col min="6916" max="6916" width="26.7109375" customWidth="1"/>
+    <col min="6917" max="6917" width="17.140625" customWidth="1"/>
+    <col min="6918" max="6918" width="57.7109375" customWidth="1"/>
+    <col min="7172" max="7172" width="26.7109375" customWidth="1"/>
+    <col min="7173" max="7173" width="17.140625" customWidth="1"/>
+    <col min="7174" max="7174" width="57.7109375" customWidth="1"/>
+    <col min="7428" max="7428" width="26.7109375" customWidth="1"/>
+    <col min="7429" max="7429" width="17.140625" customWidth="1"/>
+    <col min="7430" max="7430" width="57.7109375" customWidth="1"/>
+    <col min="7684" max="7684" width="26.7109375" customWidth="1"/>
+    <col min="7685" max="7685" width="17.140625" customWidth="1"/>
+    <col min="7686" max="7686" width="57.7109375" customWidth="1"/>
+    <col min="7940" max="7940" width="26.7109375" customWidth="1"/>
+    <col min="7941" max="7941" width="17.140625" customWidth="1"/>
+    <col min="7942" max="7942" width="57.7109375" customWidth="1"/>
+    <col min="8196" max="8196" width="26.7109375" customWidth="1"/>
+    <col min="8197" max="8197" width="17.140625" customWidth="1"/>
+    <col min="8198" max="8198" width="57.7109375" customWidth="1"/>
+    <col min="8452" max="8452" width="26.7109375" customWidth="1"/>
+    <col min="8453" max="8453" width="17.140625" customWidth="1"/>
+    <col min="8454" max="8454" width="57.7109375" customWidth="1"/>
+    <col min="8708" max="8708" width="26.7109375" customWidth="1"/>
+    <col min="8709" max="8709" width="17.140625" customWidth="1"/>
+    <col min="8710" max="8710" width="57.7109375" customWidth="1"/>
+    <col min="8964" max="8964" width="26.7109375" customWidth="1"/>
+    <col min="8965" max="8965" width="17.140625" customWidth="1"/>
+    <col min="8966" max="8966" width="57.7109375" customWidth="1"/>
+    <col min="9220" max="9220" width="26.7109375" customWidth="1"/>
+    <col min="9221" max="9221" width="17.140625" customWidth="1"/>
+    <col min="9222" max="9222" width="57.7109375" customWidth="1"/>
+    <col min="9476" max="9476" width="26.7109375" customWidth="1"/>
+    <col min="9477" max="9477" width="17.140625" customWidth="1"/>
+    <col min="9478" max="9478" width="57.7109375" customWidth="1"/>
+    <col min="9732" max="9732" width="26.7109375" customWidth="1"/>
+    <col min="9733" max="9733" width="17.140625" customWidth="1"/>
+    <col min="9734" max="9734" width="57.7109375" customWidth="1"/>
+    <col min="9988" max="9988" width="26.7109375" customWidth="1"/>
+    <col min="9989" max="9989" width="17.140625" customWidth="1"/>
+    <col min="9990" max="9990" width="57.7109375" customWidth="1"/>
+    <col min="10244" max="10244" width="26.7109375" customWidth="1"/>
+    <col min="10245" max="10245" width="17.140625" customWidth="1"/>
+    <col min="10246" max="10246" width="57.7109375" customWidth="1"/>
+    <col min="10500" max="10500" width="26.7109375" customWidth="1"/>
+    <col min="10501" max="10501" width="17.140625" customWidth="1"/>
+    <col min="10502" max="10502" width="57.7109375" customWidth="1"/>
+    <col min="10756" max="10756" width="26.7109375" customWidth="1"/>
+    <col min="10757" max="10757" width="17.140625" customWidth="1"/>
+    <col min="10758" max="10758" width="57.7109375" customWidth="1"/>
+    <col min="11012" max="11012" width="26.7109375" customWidth="1"/>
+    <col min="11013" max="11013" width="17.140625" customWidth="1"/>
+    <col min="11014" max="11014" width="57.7109375" customWidth="1"/>
+    <col min="11268" max="11268" width="26.7109375" customWidth="1"/>
+    <col min="11269" max="11269" width="17.140625" customWidth="1"/>
+    <col min="11270" max="11270" width="57.7109375" customWidth="1"/>
+    <col min="11524" max="11524" width="26.7109375" customWidth="1"/>
+    <col min="11525" max="11525" width="17.140625" customWidth="1"/>
+    <col min="11526" max="11526" width="57.7109375" customWidth="1"/>
+    <col min="11780" max="11780" width="26.7109375" customWidth="1"/>
+    <col min="11781" max="11781" width="17.140625" customWidth="1"/>
+    <col min="11782" max="11782" width="57.7109375" customWidth="1"/>
+    <col min="12036" max="12036" width="26.7109375" customWidth="1"/>
+    <col min="12037" max="12037" width="17.140625" customWidth="1"/>
+    <col min="12038" max="12038" width="57.7109375" customWidth="1"/>
+    <col min="12292" max="12292" width="26.7109375" customWidth="1"/>
+    <col min="12293" max="12293" width="17.140625" customWidth="1"/>
+    <col min="12294" max="12294" width="57.7109375" customWidth="1"/>
+    <col min="12548" max="12548" width="26.7109375" customWidth="1"/>
+    <col min="12549" max="12549" width="17.140625" customWidth="1"/>
+    <col min="12550" max="12550" width="57.7109375" customWidth="1"/>
+    <col min="12804" max="12804" width="26.7109375" customWidth="1"/>
+    <col min="12805" max="12805" width="17.140625" customWidth="1"/>
+    <col min="12806" max="12806" width="57.7109375" customWidth="1"/>
+    <col min="13060" max="13060" width="26.7109375" customWidth="1"/>
+    <col min="13061" max="13061" width="17.140625" customWidth="1"/>
+    <col min="13062" max="13062" width="57.7109375" customWidth="1"/>
+    <col min="13316" max="13316" width="26.7109375" customWidth="1"/>
+    <col min="13317" max="13317" width="17.140625" customWidth="1"/>
+    <col min="13318" max="13318" width="57.7109375" customWidth="1"/>
+    <col min="13572" max="13572" width="26.7109375" customWidth="1"/>
+    <col min="13573" max="13573" width="17.140625" customWidth="1"/>
+    <col min="13574" max="13574" width="57.7109375" customWidth="1"/>
+    <col min="13828" max="13828" width="26.7109375" customWidth="1"/>
+    <col min="13829" max="13829" width="17.140625" customWidth="1"/>
+    <col min="13830" max="13830" width="57.7109375" customWidth="1"/>
+    <col min="14084" max="14084" width="26.7109375" customWidth="1"/>
+    <col min="14085" max="14085" width="17.140625" customWidth="1"/>
+    <col min="14086" max="14086" width="57.7109375" customWidth="1"/>
+    <col min="14340" max="14340" width="26.7109375" customWidth="1"/>
+    <col min="14341" max="14341" width="17.140625" customWidth="1"/>
+    <col min="14342" max="14342" width="57.7109375" customWidth="1"/>
+    <col min="14596" max="14596" width="26.7109375" customWidth="1"/>
+    <col min="14597" max="14597" width="17.140625" customWidth="1"/>
+    <col min="14598" max="14598" width="57.7109375" customWidth="1"/>
+    <col min="14852" max="14852" width="26.7109375" customWidth="1"/>
+    <col min="14853" max="14853" width="17.140625" customWidth="1"/>
+    <col min="14854" max="14854" width="57.7109375" customWidth="1"/>
+    <col min="15108" max="15108" width="26.7109375" customWidth="1"/>
+    <col min="15109" max="15109" width="17.140625" customWidth="1"/>
+    <col min="15110" max="15110" width="57.7109375" customWidth="1"/>
+    <col min="15364" max="15364" width="26.7109375" customWidth="1"/>
+    <col min="15365" max="15365" width="17.140625" customWidth="1"/>
+    <col min="15366" max="15366" width="57.7109375" customWidth="1"/>
+    <col min="15620" max="15620" width="26.7109375" customWidth="1"/>
+    <col min="15621" max="15621" width="17.140625" customWidth="1"/>
+    <col min="15622" max="15622" width="57.7109375" customWidth="1"/>
+    <col min="15876" max="15876" width="26.7109375" customWidth="1"/>
+    <col min="15877" max="15877" width="17.140625" customWidth="1"/>
+    <col min="15878" max="15878" width="57.7109375" customWidth="1"/>
+    <col min="16132" max="16132" width="26.7109375" customWidth="1"/>
+    <col min="16133" max="16133" width="17.140625" customWidth="1"/>
+    <col min="16134" max="16134" width="57.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="47"/>
+      <c r="B3" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="47"/>
+      <c r="B4" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="46"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="46"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R63"/>
   <sheetViews>
@@ -2206,10 +2659,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="36">
         <v>42711</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>

</xml_diff>

<commit_message>
(+)    add the fun day (in prog)
</commit_message>
<xml_diff>
--- a/Suppl/Plan 2.0 - lifting.xlsx
+++ b/Suppl/Plan 2.0 - lifting.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Jan Plan '16 - r0" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
-    <sheet name="Anterior DayII" sheetId="10" r:id="rId3"/>
-    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId4"/>
+    <sheet name="Legs I" sheetId="11" r:id="rId3"/>
+    <sheet name="Anterior DayII" sheetId="10" r:id="rId4"/>
+    <sheet name="Fun Day" sheetId="12" r:id="rId5"/>
+    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$41</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="191">
   <si>
     <t>Day 1</t>
   </si>
@@ -588,6 +590,33 @@
   </si>
   <si>
     <t>3x30</t>
+  </si>
+  <si>
+    <t>Fun Day</t>
+  </si>
+  <si>
+    <t>Lying One-Arm Lateral Raise</t>
+  </si>
+  <si>
+    <t>Dumbbell Squeeze Press</t>
+  </si>
+  <si>
+    <t>Farmer's Carries</t>
+  </si>
+  <si>
+    <t>Preacher Curl 21's</t>
+  </si>
+  <si>
+    <t>Barbbell Roll Outs</t>
+  </si>
+  <si>
+    <t>Push-ups</t>
+  </si>
+  <si>
+    <t>Dumbbell Combo Walks</t>
+  </si>
+  <si>
+    <t>Plan to Push-ups</t>
   </si>
 </sst>
 </file>
@@ -674,7 +703,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,6 +725,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -831,6 +866,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -855,20 +904,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1227,10 +1272,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="44">
         <v>42711</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1276,7 +1321,7 @@
       <c r="Q4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="45" t="s">
         <v>103</v>
       </c>
       <c r="S4" t="s">
@@ -1312,7 +1357,7 @@
       <c r="Q5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R5" s="37"/>
+      <c r="R5" s="45"/>
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1329,7 +1374,7 @@
       <c r="Q6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R6" s="37"/>
+      <c r="R6" s="45"/>
       <c r="S6" t="s">
         <v>106</v>
       </c>
@@ -1349,7 +1394,7 @@
       <c r="Q7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="37" t="s">
+      <c r="R7" s="45" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1367,7 +1412,7 @@
       <c r="Q8" s="15">
         <v>3</v>
       </c>
-      <c r="R8" s="37"/>
+      <c r="R8" s="45"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1385,7 +1430,7 @@
       <c r="Q9" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R9" s="37" t="s">
+      <c r="R9" s="45" t="s">
         <v>103</v>
       </c>
       <c r="S9" t="s">
@@ -1409,7 +1454,7 @@
       <c r="Q10" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R10" s="37"/>
+      <c r="R10" s="45"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1426,7 +1471,7 @@
       <c r="Q11" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R11" s="37"/>
+      <c r="R11" s="45"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1663,20 +1708,20 @@
       <c r="Q32" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="S32" s="35" t="s">
+      <c r="S32" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
       <c r="W32" s="27"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="35"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="43"/>
+      <c r="U33" s="43"/>
+      <c r="V33" s="43"/>
       <c r="W33" s="27"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
@@ -1821,7 +1866,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,7 +1970,7 @@
       <c r="C8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="46" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="21"/>
@@ -1940,7 +1985,7 @@
       <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="21"/>
       <c r="J9" t="s">
         <v>165</v>
@@ -1953,7 +1998,7 @@
       <c r="C10" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E10" s="30" t="s">
@@ -1973,7 +2018,7 @@
       <c r="C11" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -1989,7 +2034,7 @@
       <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -2105,7 +2150,7 @@
       <c r="C28" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="30"/>
@@ -2123,7 +2168,7 @@
       <c r="C29" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="47"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2139,7 +2184,7 @@
       <c r="C30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E30" s="30"/>
@@ -2157,7 +2202,7 @@
       <c r="C31" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="38"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -2173,7 +2218,7 @@
       <c r="C32" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="30"/>
@@ -2191,24 +2236,24 @@
       <c r="C33" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="38"/>
-      <c r="E33" s="41" t="s">
+      <c r="D33" s="46"/>
+      <c r="E33" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
       <c r="J33" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C34" s="18"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -2217,7 +2262,7 @@
       <c r="C35" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="46" t="s">
         <v>103</v>
       </c>
       <c r="E35" s="21" t="s">
@@ -2237,7 +2282,7 @@
       <c r="C36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -2301,10 +2346,186 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="J2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="J3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="J4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="J5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="J6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="19">
+        <v>3</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="21"/>
+      <c r="J7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="J8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="J9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="J10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,122 +2725,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="46"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="38" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="49" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="38" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="49" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="38" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="50" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="38" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="49" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="41" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="48" t="s">
+    <row r="7" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="49" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="41" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="46"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="46"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
+      <c r="A10" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="52"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="55"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="53"/>
+      <c r="B5" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="55"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="53"/>
+      <c r="B6" s="54" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="53"/>
+      <c r="B7" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="53"/>
+      <c r="B8" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="53"/>
+      <c r="B9" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="53"/>
+      <c r="B10" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R63"/>
   <sheetViews>
@@ -2659,10 +2983,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="44">
         <v>42711</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>

</xml_diff>

<commit_message>
(+)    add new Rob notes
</commit_message>
<xml_diff>
--- a/Suppl/Plan 2.0 - lifting.xlsx
+++ b/Suppl/Plan 2.0 - lifting.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jan Plan '16 - r0" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
-    <sheet name="Legs I" sheetId="11" r:id="rId3"/>
-    <sheet name="Anterior DayII" sheetId="10" r:id="rId4"/>
-    <sheet name="Fun Day" sheetId="12" r:id="rId5"/>
-    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId6"/>
+    <sheet name="Posterior Day I" sheetId="13" r:id="rId3"/>
+    <sheet name="Legs I" sheetId="11" r:id="rId4"/>
+    <sheet name="Anterior DayII" sheetId="10" r:id="rId5"/>
+    <sheet name="Fun Day" sheetId="12" r:id="rId6"/>
+    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$41</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="200">
   <si>
     <t>Day 1</t>
   </si>
@@ -617,6 +618,33 @@
   </si>
   <si>
     <t>Plan to Push-ups</t>
+  </si>
+  <si>
+    <t>Resistance against gravity</t>
+  </si>
+  <si>
+    <t>Underhand Lat Pull-down</t>
+  </si>
+  <si>
+    <t>Banded Good Mornings</t>
+  </si>
+  <si>
+    <t>Row Machine, Wide Grip</t>
+  </si>
+  <si>
+    <t>Rear Delt Fly, Isometric with Back Extension</t>
+  </si>
+  <si>
+    <t>Bent-over row, underhand grips</t>
+  </si>
+  <si>
+    <t>Heavy Bicep Curl, your choice</t>
+  </si>
+  <si>
+    <t>3x60s</t>
+  </si>
+  <si>
+    <t>3x8-12</t>
   </si>
 </sst>
 </file>
@@ -703,7 +731,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,6 +759,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -880,6 +914,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -904,16 +948,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,10 +1310,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="50">
         <v>42711</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1321,7 +1359,7 @@
       <c r="Q4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="R4" s="45" t="s">
+      <c r="R4" s="51" t="s">
         <v>103</v>
       </c>
       <c r="S4" t="s">
@@ -1357,7 +1395,7 @@
       <c r="Q5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R5" s="45"/>
+      <c r="R5" s="51"/>
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1374,7 +1412,7 @@
       <c r="Q6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R6" s="45"/>
+      <c r="R6" s="51"/>
       <c r="S6" t="s">
         <v>106</v>
       </c>
@@ -1394,7 +1432,7 @@
       <c r="Q7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="45" t="s">
+      <c r="R7" s="51" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1412,7 +1450,7 @@
       <c r="Q8" s="15">
         <v>3</v>
       </c>
-      <c r="R8" s="45"/>
+      <c r="R8" s="51"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1430,7 +1468,7 @@
       <c r="Q9" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R9" s="45" t="s">
+      <c r="R9" s="51" t="s">
         <v>103</v>
       </c>
       <c r="S9" t="s">
@@ -1454,7 +1492,7 @@
       <c r="Q10" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R10" s="45"/>
+      <c r="R10" s="51"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1471,7 +1509,7 @@
       <c r="Q11" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R11" s="45"/>
+      <c r="R11" s="51"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1708,20 +1746,20 @@
       <c r="Q32" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="S32" s="43" t="s">
+      <c r="S32" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="T32" s="43"/>
-      <c r="U32" s="43"/>
-      <c r="V32" s="43"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="49"/>
+      <c r="V32" s="49"/>
       <c r="W32" s="27"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="S33" s="43"/>
-      <c r="T33" s="43"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="43"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="49"/>
       <c r="W33" s="27"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
@@ -1865,8 +1903,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:M12"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +2008,7 @@
       <c r="C8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="52" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="21"/>
@@ -1985,7 +2023,7 @@
       <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="21"/>
       <c r="J9" t="s">
         <v>165</v>
@@ -1998,7 +2036,7 @@
       <c r="C10" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E10" s="30" t="s">
@@ -2018,7 +2056,7 @@
       <c r="C11" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -2034,7 +2072,7 @@
       <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="47"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -2150,7 +2188,7 @@
       <c r="C28" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="30"/>
@@ -2168,7 +2206,7 @@
       <c r="C29" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2184,7 +2222,7 @@
       <c r="C30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E30" s="30"/>
@@ -2202,7 +2240,7 @@
       <c r="C31" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="46"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -2218,7 +2256,7 @@
       <c r="C32" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="30"/>
@@ -2236,24 +2274,24 @@
       <c r="C33" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="46"/>
-      <c r="E33" s="49" t="s">
+      <c r="D33" s="52"/>
+      <c r="E33" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
       <c r="J33" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C34" s="18"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -2262,7 +2300,7 @@
       <c r="C35" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="52" t="s">
         <v>103</v>
       </c>
       <c r="E35" s="21" t="s">
@@ -2282,7 +2320,7 @@
       <c r="C36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="47"/>
+      <c r="D36" s="53"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -2346,6 +2384,114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="A2:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+      <c r="B4" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="58" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="57"/>
+      <c r="B6" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="58" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
+      <c r="B8" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2353,6 +2499,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
@@ -2438,7 +2587,7 @@
       <c r="C6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="52" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="21"/>
@@ -2453,7 +2602,7 @@
       <c r="C7" s="19">
         <v>3</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="21"/>
       <c r="J7" t="s">
         <v>165</v>
@@ -2466,7 +2615,7 @@
       <c r="C8" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="30" t="s">
@@ -2486,7 +2635,7 @@
       <c r="C9" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -2502,7 +2651,7 @@
       <c r="C10" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -2520,7 +2669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2840,11 +2989,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E10"/>
     </sheetView>
   </sheetViews>
@@ -2862,94 +3011,92 @@
       <c r="B2" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="54" t="s">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="55"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="55"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="56" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="55"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="47"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="56" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2983,10 +3130,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="50">
         <v>42711</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>

</xml_diff>

<commit_message>
(C)    Fun Day Updates
</commit_message>
<xml_diff>
--- a/Suppl/Plan 2.0 - lifting.xlsx
+++ b/Suppl/Plan 2.0 - lifting.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Jan Plan '16 - r0" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="208">
   <si>
     <t>Day 1</t>
   </si>
@@ -645,6 +645,30 @@
   </si>
   <si>
     <t>3x8-12</t>
+  </si>
+  <si>
+    <t>(Bodyweight Pushup, Floor Regular)</t>
+  </si>
+  <si>
+    <t>(Lying One-Arm Lateral Raise)</t>
+  </si>
+  <si>
+    <t>(Lying Dumbbell Squeeze Press)</t>
+  </si>
+  <si>
+    <t>(Walking Farmer's Carries)</t>
+  </si>
+  <si>
+    <t>(Preacher Curl 21's)</t>
+  </si>
+  <si>
+    <t>(Barbell Roll-outs, Floor)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Combo Walks, Fat Gripz)</t>
+  </si>
+  <si>
+    <t>(Plank to Push-up)</t>
   </si>
 </sst>
 </file>
@@ -924,6 +948,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -947,10 +975,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1310,10 +1334,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="50">
+      <c r="B2" s="52">
         <v>42711</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1359,7 +1383,7 @@
       <c r="Q4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="R4" s="53" t="s">
         <v>103</v>
       </c>
       <c r="S4" t="s">
@@ -1395,7 +1419,7 @@
       <c r="Q5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R5" s="51"/>
+      <c r="R5" s="53"/>
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1412,7 +1436,7 @@
       <c r="Q6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R6" s="51"/>
+      <c r="R6" s="53"/>
       <c r="S6" t="s">
         <v>106</v>
       </c>
@@ -1432,7 +1456,7 @@
       <c r="Q7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="51" t="s">
+      <c r="R7" s="53" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1450,7 +1474,7 @@
       <c r="Q8" s="15">
         <v>3</v>
       </c>
-      <c r="R8" s="51"/>
+      <c r="R8" s="53"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1468,7 +1492,7 @@
       <c r="Q9" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="R9" s="51" t="s">
+      <c r="R9" s="53" t="s">
         <v>103</v>
       </c>
       <c r="S9" t="s">
@@ -1492,7 +1516,7 @@
       <c r="Q10" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R10" s="51"/>
+      <c r="R10" s="53"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1509,7 +1533,7 @@
       <c r="Q11" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="R11" s="51"/>
+      <c r="R11" s="53"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1746,20 +1770,20 @@
       <c r="Q32" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="S32" s="49" t="s">
+      <c r="S32" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="T32" s="49"/>
-      <c r="U32" s="49"/>
-      <c r="V32" s="49"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="51"/>
+      <c r="V32" s="51"/>
       <c r="W32" s="27"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="49"/>
-      <c r="V33" s="49"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="51"/>
       <c r="W33" s="27"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
@@ -2008,7 +2032,7 @@
       <c r="C8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="21"/>
@@ -2023,7 +2047,7 @@
       <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="21"/>
       <c r="J9" t="s">
         <v>165</v>
@@ -2036,7 +2060,7 @@
       <c r="C10" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="56" t="s">
         <v>103</v>
       </c>
       <c r="E10" s="30" t="s">
@@ -2056,7 +2080,7 @@
       <c r="C11" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="52"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -2072,7 +2096,7 @@
       <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -2188,7 +2212,7 @@
       <c r="C28" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="56" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="30"/>
@@ -2206,7 +2230,7 @@
       <c r="C29" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="53"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2222,7 +2246,7 @@
       <c r="C30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D30" s="56" t="s">
         <v>103</v>
       </c>
       <c r="E30" s="30"/>
@@ -2240,7 +2264,7 @@
       <c r="C31" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="52"/>
+      <c r="D31" s="54"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -2256,7 +2280,7 @@
       <c r="C32" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="56" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="30"/>
@@ -2274,24 +2298,24 @@
       <c r="C33" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="52"/>
-      <c r="E33" s="55" t="s">
+      <c r="D33" s="54"/>
+      <c r="E33" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
       <c r="J33" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C34" s="18"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -2300,7 +2324,7 @@
       <c r="C35" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E35" s="21" t="s">
@@ -2320,7 +2344,7 @@
       <c r="C36" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="53"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -2386,7 +2410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
@@ -2409,79 +2433,79 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="58" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58" t="s">
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="58" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="58" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57" t="s">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="58" t="s">
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="50" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="57" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58" t="s">
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2587,7 +2611,7 @@
       <c r="C6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="54" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="21"/>
@@ -2602,7 +2626,7 @@
       <c r="C7" s="19">
         <v>3</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="21"/>
       <c r="J7" t="s">
         <v>165</v>
@@ -2615,7 +2639,7 @@
       <c r="C8" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="56" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="30" t="s">
@@ -2635,7 +2659,7 @@
       <c r="C9" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -2651,7 +2675,7 @@
       <c r="C10" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="53"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -2991,20 +3015,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="4.140625" style="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>98</v>
       </c>
@@ -3015,7 +3042,7 @@
       <c r="D2" s="43"/>
       <c r="E2" s="44"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="45"/>
       <c r="B3" s="46" t="s">
         <v>183</v>
@@ -3023,8 +3050,11 @@
       <c r="C3" s="45"/>
       <c r="D3" s="45"/>
       <c r="E3" s="47"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="46" t="s">
         <v>184</v>
@@ -3032,8 +3062,11 @@
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
       <c r="E4" s="47"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="48" t="s">
         <v>185</v>
@@ -3041,8 +3074,11 @@
       <c r="C5" s="48"/>
       <c r="D5" s="45"/>
       <c r="E5" s="47"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="46" t="s">
         <v>186</v>
@@ -3050,8 +3086,11 @@
       <c r="C6" s="45"/>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="46" t="s">
         <v>187</v>
@@ -3059,8 +3098,11 @@
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="48" t="s">
         <v>188</v>
@@ -3068,8 +3110,11 @@
       <c r="C8" s="48"/>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="46" t="s">
         <v>189</v>
@@ -3077,8 +3122,11 @@
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="46" t="s">
         <v>190</v>
@@ -3086,6 +3134,9 @@
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
+      <c r="G10" t="s">
+        <v>207</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3130,10 +3181,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="50">
+      <c r="B2" s="52">
         <v>42711</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>

</xml_diff>

<commit_message>
(U)    Posterior workout update, swapped to Front Pulldowns
</commit_message>
<xml_diff>
--- a/Suppl/Plan 2.0 - lifting.xlsx
+++ b/Suppl/Plan 2.0 - lifting.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jan Plan '16 - r0" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Legs I" sheetId="11" r:id="rId4"/>
     <sheet name="Anterior DayII" sheetId="10" r:id="rId5"/>
     <sheet name="Fun Day" sheetId="12" r:id="rId6"/>
-    <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$41</definedName>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="147">
   <si>
     <t>Day 1</t>
   </si>
@@ -47,12 +46,6 @@
     <t>Day 4</t>
   </si>
   <si>
-    <t>Lateral Raise</t>
-  </si>
-  <si>
-    <t>Crunches</t>
-  </si>
-  <si>
     <t>Plan</t>
   </si>
   <si>
@@ -68,120 +61,12 @@
     <t>Get started with trainer's routine</t>
   </si>
   <si>
-    <t>Shoulders/Triceps ()</t>
-  </si>
-  <si>
-    <t>Back/Biceps ()</t>
-  </si>
-  <si>
-    <t>Chest/Abs ()</t>
-  </si>
-  <si>
-    <t>Legs ()</t>
-  </si>
-  <si>
-    <t>Lateral Pulldown</t>
-  </si>
-  <si>
-    <t>Seated Hammer Strength Rows</t>
-  </si>
-  <si>
-    <t>Close Grip Pulldown</t>
-  </si>
-  <si>
-    <t>*(Wide, Overhand, Narrow)</t>
-  </si>
-  <si>
-    <t>Individual Incline Dumbbell Curls</t>
-  </si>
-  <si>
-    <t>Alternating Individual Dumbbell Bicep Curls</t>
-  </si>
-  <si>
-    <t>Seated Individual Single Arm Cable Rows</t>
-  </si>
-  <si>
-    <t>Inclline Dumbbell Press</t>
-  </si>
-  <si>
-    <t>Flat Bench Dumbbell Press</t>
-  </si>
-  <si>
-    <t>Individual Single Leg Extension</t>
-  </si>
-  <si>
-    <t>Individual Weighted Step-Ups</t>
-  </si>
-  <si>
-    <t>Seated Hamstring Curls</t>
-  </si>
-  <si>
-    <t>Individual Leg Hamstring Curls</t>
-  </si>
-  <si>
-    <t>Dumbbell Front Raise</t>
-  </si>
-  <si>
-    <t>Seated Dumbbell Shoulder Press</t>
-  </si>
-  <si>
-    <t>Cable Face Pulls</t>
-  </si>
-  <si>
-    <t>Cable Rope Pushdowns</t>
-  </si>
-  <si>
-    <t>Close-Grip Bench Push-Ups</t>
-  </si>
-  <si>
-    <t>Seated Dip Machine</t>
-  </si>
-  <si>
-    <t>4x15</t>
-  </si>
-  <si>
-    <t>4x12</t>
-  </si>
-  <si>
-    <t>4x10</t>
-  </si>
-  <si>
-    <t>4x8</t>
-  </si>
-  <si>
-    <t>1 min</t>
-  </si>
-  <si>
-    <t>Flutter Kicks</t>
-  </si>
-  <si>
-    <t>Ab Circuit</t>
-  </si>
-  <si>
-    <t>Leg Lifts</t>
-  </si>
-  <si>
     <t>Plank</t>
   </si>
   <si>
-    <t>Russian Twists</t>
-  </si>
-  <si>
     <t>3x12</t>
   </si>
   <si>
-    <t>3x10</t>
-  </si>
-  <si>
-    <t>3x8</t>
-  </si>
-  <si>
-    <t>3x16</t>
-  </si>
-  <si>
-    <t>4xFail</t>
-  </si>
-  <si>
     <t>4 Days Lift, 1 Day Cardio, 1 Day Rest</t>
   </si>
   <si>
@@ -194,21 +79,6 @@
     <t>Post</t>
   </si>
   <si>
-    <t>4x15 ea.</t>
-  </si>
-  <si>
-    <t>Machine Butterfly</t>
-  </si>
-  <si>
-    <t>Cable Crossover Fly</t>
-  </si>
-  <si>
-    <t>Lunges</t>
-  </si>
-  <si>
-    <t>Single Leg No-Weight Calf Raise</t>
-  </si>
-  <si>
     <t>15 min Elliptical (15/15)</t>
   </si>
   <si>
@@ -221,97 +91,16 @@
     <t>Life Fitness Buddy Names</t>
   </si>
   <si>
-    <t>(12/7/16) r2</t>
-  </si>
-  <si>
-    <t>(Lateral Pulldown)</t>
-  </si>
-  <si>
     <t>(Seated Hammer Strength Rows)</t>
   </si>
   <si>
-    <t>(Close Grip Pulldown)</t>
-  </si>
-  <si>
-    <t>(Seated Individual Arm Cable Rows)</t>
-  </si>
-  <si>
     <t>(Alternating Individual Dumbbell Bicep Curls)</t>
   </si>
   <si>
-    <t>(Barbbell Preacher Curls)</t>
-  </si>
-  <si>
-    <t>Barbbell Preacher Curls</t>
-  </si>
-  <si>
-    <t>(Individual Incline Dumbbell Curls)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Bench Press - Incline)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Bench Press - Flat)</t>
-  </si>
-  <si>
-    <t>(Cable Crossover - High)</t>
-  </si>
-  <si>
-    <t>(Selectorized Fly)</t>
-  </si>
-  <si>
-    <t>(Bodyweight Crunch)</t>
-  </si>
-  <si>
-    <t>(Bodyweight Leg Raise)</t>
-  </si>
-  <si>
     <t>(Bodyweight Plank)</t>
   </si>
   <si>
-    <t>(Bodyweight Twist - Russian)</t>
-  </si>
-  <si>
-    <t>(Flutter Kick)</t>
-  </si>
-  <si>
     <t>(Selectorized Individual Leg Extension)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Step Up - Platform)</t>
-  </si>
-  <si>
-    <t>(Selectorized Leg Curl)</t>
-  </si>
-  <si>
-    <t>(Selectorized Individual Leg Curl)</t>
-  </si>
-  <si>
-    <t>(Bodyweight Lunge)</t>
-  </si>
-  <si>
-    <t>(Stair Bodyweight Calf Raise)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Raise - Front)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Raise - Lateral)</t>
-  </si>
-  <si>
-    <t>(Selectorized Shoulder Press - Overhand)</t>
-  </si>
-  <si>
-    <t>(Cable Face Pull)</t>
-  </si>
-  <si>
-    <t>(Cable Pushdown - Overhand)</t>
-  </si>
-  <si>
-    <t>(Close-Grip Bench Push-Ups)</t>
-  </si>
-  <si>
-    <t>(Seated Dip)</t>
   </si>
   <si>
     <t>(1/4/16) r0</t>
@@ -669,6 +458,33 @@
   </si>
   <si>
     <t>(Plank to Push-up)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>previous first lift was Underhand Lat Pull-down, replaced with Front Pulldown by Justin because he likes the machine and the input of the lift more for his routine</t>
+  </si>
+  <si>
+    <t>(Lateral Pulldown, Underhand Grip)</t>
+  </si>
+  <si>
+    <t>(Barbbell Good Morning)</t>
+  </si>
+  <si>
+    <t>(Bent Over Barbbell Row, Underhand with Drag)</t>
+  </si>
+  <si>
+    <t>Orig: Lateral Pulldown, Underhand Grip</t>
+  </si>
+  <si>
+    <t>New: Front Pulldown</t>
+  </si>
+  <si>
+    <t>Selectorized Front Puldown, Underhand Grip</t>
+  </si>
+  <si>
+    <t>Lats, Biceps, Rear Deltoids</t>
   </si>
 </sst>
 </file>
@@ -1311,28 +1127,28 @@
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="52">
         <v>42711</v>
@@ -1342,33 +1158,33 @@
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
       <c r="O3" s="23" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1378,16 +1194,16 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
       <c r="P4" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="R4" s="53" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="S4" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
@@ -1395,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
@@ -1405,19 +1221,19 @@
         <v>2</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="7"/>
       <c r="K5" s="22" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="L5" s="21"/>
       <c r="P5" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="R5" s="53"/>
     </row>
@@ -1431,14 +1247,14 @@
       <c r="J6" s="10"/>
       <c r="K6" s="15"/>
       <c r="P6" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="R6" s="53"/>
       <c r="S6" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1451,13 +1267,13 @@
       <c r="J7" s="11"/>
       <c r="K7" s="15"/>
       <c r="P7" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="R7" s="53" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1469,7 +1285,7 @@
       <c r="G8" s="2"/>
       <c r="K8" s="15"/>
       <c r="P8" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="Q8" s="15">
         <v>3</v>
@@ -1487,16 +1303,16 @@
       <c r="J9" s="11"/>
       <c r="K9" s="15"/>
       <c r="P9" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="R9" s="53" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="S9" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1511,10 +1327,10 @@
       <c r="J10" s="11"/>
       <c r="K10" s="15"/>
       <c r="P10" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="R10" s="53"/>
     </row>
@@ -1528,10 +1344,10 @@
       <c r="H11" s="2"/>
       <c r="K11" s="15"/>
       <c r="P11" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="R11" s="53"/>
     </row>
@@ -1544,7 +1360,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="O12" s="23" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1555,7 +1371,7 @@
       <c r="F13" s="15"/>
       <c r="K13" s="15"/>
       <c r="P13" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
@@ -1565,7 +1381,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="P14" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
@@ -1573,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -1583,18 +1399,18 @@
         <v>3</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="7"/>
       <c r="K15" s="18"/>
       <c r="O15" s="23" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="2"/>
@@ -1603,7 +1419,7 @@
       <c r="H16" s="14"/>
       <c r="K16" s="15"/>
       <c r="P16" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1615,7 +1431,7 @@
       <c r="H17" s="14"/>
       <c r="K17" s="15"/>
       <c r="O17" s="23" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1627,7 +1443,7 @@
       <c r="H18" s="14"/>
       <c r="K18" s="15"/>
       <c r="P18" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="12"/>
@@ -1641,7 +1457,7 @@
       <c r="H19" s="14"/>
       <c r="K19" s="15"/>
       <c r="P19" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1653,10 +1469,10 @@
       <c r="H20" s="14"/>
       <c r="K20" s="15"/>
       <c r="P20" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -1668,7 +1484,7 @@
       <c r="H21" s="14"/>
       <c r="K21" s="15"/>
       <c r="P21" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -1693,15 +1509,15 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="O24" s="28" t="s">
-        <v>130</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -1716,62 +1532,62 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="O26" s="23" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P27" t="s">
-        <v>131</v>
+        <v>61</v>
       </c>
       <c r="Q27" s="15" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P28" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="Q28" s="15" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P29" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="Q29" s="15" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P30" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="Q30" s="15" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="P31" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
       <c r="Q31" s="15" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="P32" t="s">
-        <v>136</v>
+        <v>66</v>
       </c>
       <c r="Q32" s="15" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="S32" s="51" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="T32" s="51"/>
       <c r="U32" s="51"/>
@@ -1789,13 +1605,13 @@
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="P34" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="Q34" s="15" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="S34" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="T34" s="26"/>
       <c r="U34" s="26"/>
@@ -1805,42 +1621,42 @@
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="P35" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="Q35" s="15" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="O36" s="23" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="P37" s="11" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38" s="20"/>
       <c r="O38" s="23" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="2"/>
       <c r="P39" s="11" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40" s="14"/>
       <c r="C40" s="2"/>
       <c r="P40" s="11" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
@@ -1904,7 +1720,7 @@
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J63" s="9" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1940,7 +1756,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="C1" s="15"/>
     </row>
@@ -1949,7 +1765,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="21"/>
@@ -1957,92 +1773,92 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="J5" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="21" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="J6" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="D7" s="33"/>
       <c r="E7" s="6" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="J7" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E8" s="21"/>
       <c r="J8" t="s">
-        <v>169</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="C9" s="19">
         <v>3</v>
@@ -2050,35 +1866,35 @@
       <c r="D9" s="54"/>
       <c r="E9" s="21"/>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
       <c r="J10" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="D11" s="54"/>
       <c r="E11" s="21"/>
@@ -2086,15 +1902,15 @@
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="J11" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="D12" s="55"/>
       <c r="E12" s="6"/>
@@ -2102,30 +1918,30 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="J12" t="s">
-        <v>167</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="C16" s="15"/>
       <c r="F16">
@@ -2134,7 +1950,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="C17" s="15"/>
       <c r="F17">
@@ -2144,7 +1960,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15"/>
       <c r="F18" s="34">
@@ -2154,7 +1970,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="12"/>
@@ -2165,22 +1981,22 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="C21" s="15"/>
       <c r="E21" s="17" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
       <c r="C22" s="15"/>
     </row>
@@ -2192,7 +2008,7 @@
     </row>
     <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="C25" s="15"/>
     </row>
@@ -2201,34 +2017,34 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>131</v>
+        <v>61</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="D28" s="56" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
       <c r="H28" s="30"/>
       <c r="J28" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="D29" s="55"/>
       <c r="E29" s="6"/>
@@ -2236,33 +2052,33 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="J29" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="D30" s="56" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
       <c r="H30" s="30"/>
       <c r="J30" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="D31" s="54"/>
       <c r="E31" s="21"/>
@@ -2270,43 +2086,43 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="J31" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="D32" s="56" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
       <c r="H32" s="30"/>
       <c r="J32" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>136</v>
+        <v>66</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="57" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="F33" s="57"/>
       <c r="G33" s="57"/>
       <c r="H33" s="57"/>
       <c r="J33" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2319,30 +2135,30 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="D35" s="54" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="J35" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="D36" s="55"/>
       <c r="E36" s="6"/>
@@ -2350,35 +2166,35 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="J36" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="C37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="C41" s="15"/>
     </row>
@@ -2408,109 +2224,165 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="A2:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" activeCellId="1" sqref="G20 H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
       <c r="E1" s="37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49"/>
       <c r="B2" s="49" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="B3" s="49" t="s">
-        <v>193</v>
+        <v>123</v>
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="49"/>
       <c r="B4" s="49" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="49"/>
       <c r="E4" s="50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>195</v>
+        <v>125</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="49"/>
       <c r="E5" s="50" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
       <c r="B6" s="49" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
       <c r="E6" s="50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
       <c r="B7" s="49" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
       <c r="E7" s="50" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
       <c r="B8" s="49" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
       <c r="E8" s="50" t="s">
-        <v>198</v>
+        <v>128</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2529,7 +2401,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="21"/>
@@ -2537,91 +2409,91 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="J3" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="21" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="J4" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="6" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="J5" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E6" s="21"/>
       <c r="J6" t="s">
-        <v>169</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="C7" s="19">
         <v>3</v>
@@ -2629,35 +2501,35 @@
       <c r="D7" s="54"/>
       <c r="E7" s="21"/>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="J8" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="D9" s="54"/>
       <c r="E9" s="21"/>
@@ -2665,15 +2537,15 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="J9" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="6"/>
@@ -2681,7 +2553,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="J10" t="s">
-        <v>167</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2902,91 +2774,91 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
       <c r="E1" s="37" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="40" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="41" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="40" t="s">
-        <v>174</v>
+        <v>104</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="41" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="40" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="41" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
       <c r="B5" s="40" t="s">
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="42" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
       <c r="B6" s="40" t="s">
-        <v>178</v>
+        <v>108</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="41" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39"/>
       <c r="B7" s="40" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="41" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3017,7 +2889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3028,15 +2900,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="43"/>
@@ -3045,791 +2917,100 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="45"/>
       <c r="B3" s="46" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
       <c r="C3" s="45"/>
       <c r="D3" s="45"/>
       <c r="E3" s="47"/>
       <c r="G3" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="46" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
       <c r="E4" s="47"/>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="48" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="45"/>
       <c r="E5" s="47"/>
       <c r="G5" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="46" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
       <c r="C6" s="45"/>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
       <c r="G6" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="46" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
       <c r="G7" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="48" t="s">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
       <c r="G8" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="46" t="s">
-        <v>189</v>
+        <v>119</v>
       </c>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
       <c r="G9" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="46" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
       <c r="G10" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R63"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.5703125" style="17" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="52">
-        <v>42711</v>
-      </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="21"/>
-    </row>
-    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="E6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="H6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="E7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="2"/>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="2"/>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="E9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="E10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="E11" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="E12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="E13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="2"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="E16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="H16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="E17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="H17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="E18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="15"/>
-      <c r="H18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="15"/>
-      <c r="H19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="E20" s="15">
-        <v>5</v>
-      </c>
-      <c r="F20" s="15"/>
-      <c r="H20" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="15">
-        <v>20</v>
-      </c>
-      <c r="F21" s="15"/>
-      <c r="H21" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="15">
-        <v>20</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="H22" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="H23" s="14"/>
-      <c r="K23" s="15"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="15">
-        <v>40</v>
-      </c>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="15">
-        <v>40</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="F39" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="F40" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="F41" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>26</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J63" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>